<commit_message>
update file checklist_security-lab3 in security branch
</commit_message>
<xml_diff>
--- a/security/checklist_security-lab3.xlsx
+++ b/security/checklist_security-lab3.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Tên project</t>
   </si>
@@ -487,6 +487,9 @@
 - Login bod, paste link đã copy =&gt; không thể thực hiện được
 - Login bod, click vào link delete của test =&gt; có thể thực hiện được</t>
   </si>
+  <si>
+    <t>NG</t>
+  </si>
 </sst>
 </file>
 
@@ -729,16 +732,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1905,9 +1908,9 @@
   <dimension ref="A1:AE898"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomLeft" activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4363636363636" defaultRowHeight="15.75" customHeight="1"/>
@@ -2457,7 +2460,9 @@
       <c r="Y13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="Z13" s="25"/>
+      <c r="Z13" s="25" t="s">
+        <v>34</v>
+      </c>
       <c r="AA13" s="25"/>
       <c r="AB13" s="25"/>
       <c r="AC13" s="25"/>

</xml_diff>